<commit_message>
Spreadsheet update, minor code changes
Updated the spreadsheet to separate the creator tag and potential card sets (Main 1, Main 2, Aux 1, Aux 2, etc)

Modified the positions of the creator tag, version NO, and card names in the script.
</commit_message>
<xml_diff>
--- a/Main/Compile_HomebrewData_Template.xlsx
+++ b/Main/Compile_HomebrewData_Template.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Protocol Name</t>
   </si>
@@ -23,6 +23,9 @@
     <t>Protocol Actions</t>
   </si>
   <si>
+    <t>Pack</t>
+  </si>
+  <si>
     <t>Creator Tag</t>
   </si>
   <si>
@@ -53,14 +56,23 @@
     <t>Auxiliary Text</t>
   </si>
   <si>
-    <t>v0.1</t>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>Persistent</t>
+  </si>
+  <si>
+    <t>Immediate</t>
+  </si>
+  <si>
+    <t>Auxiliary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -71,6 +83,12 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="24.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -80,9 +98,22 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border/>
     <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -104,21 +135,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -126,17 +157,42 @@
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" textRotation="90" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -361,7 +417,7 @@
     <col customWidth="1" min="1" max="1" width="15.75"/>
     <col customWidth="1" min="2" max="2" width="31.38"/>
     <col customWidth="1" min="3" max="3" width="25.13"/>
-    <col customWidth="1" min="4" max="4" width="14.38"/>
+    <col customWidth="1" min="4" max="5" width="14.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -377,12 +433,16 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -397,127 +457,158 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75" outlineLevelCol="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="6.5"/>
-    <col customWidth="1" min="2" max="2" width="20.5"/>
-    <col customWidth="1" min="3" max="3" width="5.13"/>
-    <col customWidth="1" min="4" max="4" width="18.88"/>
-    <col customWidth="1" min="5" max="5" width="28.25"/>
-    <col customWidth="1" min="6" max="6" width="18.88"/>
-    <col customWidth="1" min="7" max="7" width="28.25"/>
-    <col customWidth="1" min="8" max="8" width="18.88"/>
-    <col customWidth="1" min="9" max="9" width="28.25"/>
+    <col customWidth="1" min="1" max="1" width="5.5"/>
+    <col customWidth="1" min="2" max="2" width="6.5" outlineLevel="1"/>
+    <col customWidth="1" min="3" max="3" width="9.5" outlineLevel="1"/>
+    <col customWidth="1" min="4" max="4" width="5.13"/>
+    <col customWidth="1" min="5" max="5" width="5.5"/>
+    <col customWidth="1" min="6" max="7" width="27.0" outlineLevel="1"/>
+    <col customWidth="1" min="8" max="8" width="5.5"/>
+    <col customWidth="1" min="9" max="10" width="27.0" outlineLevel="1"/>
+    <col customWidth="1" min="11" max="11" width="5.5"/>
+    <col customWidth="1" min="12" max="13" width="27.0" outlineLevel="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="7"/>
+      <c r="L1" s="8" t="s">
         <v>12</v>
       </c>
+      <c r="M1" s="8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="9"/>
+      <c r="A2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="14"/>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="7"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="E2:E7"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="K2:K7"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>